<commit_message>
Download Excel file Remaining
</commit_message>
<xml_diff>
--- a/InvoiceData.xlsx
+++ b/InvoiceData.xlsx
@@ -1,52 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
-  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Robots\Robot3\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050" firstSheet="0" activeTab="0"/>
+    <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <x:sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="0"/>
+  <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <x:si>
-    <x:t>FKAR211307968617</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1565.0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2022-12-01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>LKO1-2440918</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1548.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2022-10-01</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0130253080700006</x:t>
-  </x:si>
-  <x:si>
-    <x:t>31.50</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2022-08-07</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <x:si>
+    <x:t>2170</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1725.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-09-29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3031</x:t>
+  </x:si>
+  <x:si>
+    <x:t>650.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2016-10-27</x:t>
   </x:si>
   <x:si>
     <x:t>22IF5N8B00032780</x:t>
@@ -61,12 +46,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2">
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1" x14ac:knownFonts="1">
+  <x:fonts count="1">
     <x:font>
+      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -82,32 +68,38 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
   <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
 </x:styleSheet>
 </file>
 
@@ -395,20 +387,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C8"/>
+  <x:dimension ref="A1:C1"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0"/>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <x:cols>
-    <x:col min="1" max="1" width="17.855469" style="0" bestFit="1" customWidth="1"/>
-  </x:cols>
+  <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:3">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -419,7 +408,7 @@
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="2" spans="1:3">
       <x:c r="A2" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -430,7 +419,7 @@
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="3" spans="1:3">
       <x:c r="A3" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
@@ -441,7 +430,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="4" spans="1:3">
       <x:c r="A4" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
@@ -452,7 +441,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="5" spans="1:3">
       <x:c r="A5" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -463,7 +452,7 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="6" spans="1:3">
       <x:c r="A6" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -474,290 +463,70 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="7" spans="1:3">
       <x:c r="A7" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:3">
       <x:c r="A8" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3">
       <x:c r="A9" s="0" t="s">
-        <x:v>0</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3">
       <x:c r="A10" s="0" t="s">
-        <x:v>0</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3">
       <x:c r="A11" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:3">
       <x:c r="A12" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:3">
-      <x:c r="A13" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B13" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C13" s="0" t="s">
         <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:3">
-      <x:c r="A14" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B14" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C14" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:3">
-      <x:c r="A15" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B15" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C15" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:3">
-      <x:c r="A16" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B16" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C16" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:3">
-      <x:c r="A17" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B17" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C17" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:3">
-      <x:c r="A18" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B18" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C18" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:3">
-      <x:c r="A19" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B19" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C19" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:3">
-      <x:c r="A20" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B20" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C20" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:3">
-      <x:c r="A21" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B21" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C21" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="22" spans="1:3">
-      <x:c r="A22" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B22" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C22" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:3">
-      <x:c r="A23" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B23" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C23" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="24" spans="1:3">
-      <x:c r="A24" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B24" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C24" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="25" spans="1:3">
-      <x:c r="A25" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B25" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C25" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:3">
-      <x:c r="A26" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B26" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C26" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:3">
-      <x:c r="A27" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B27" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C27" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:3">
-      <x:c r="A28" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B28" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C28" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:3">
-      <x:c r="A29" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B29" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C29" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="30" spans="1:3">
-      <x:c r="A30" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B30" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C30" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="1:3">
-      <x:c r="A31" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B31" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C31" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:3">
-      <x:c r="A32" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B32" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C32" s="0" t="s">
-        <x:v>11</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>